<commit_message>
player movement - first commit
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F418D78-9B96-4E6C-A3A9-D6C5EC5108E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544DC3E9-8281-4935-B92A-A62AE4DFD7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -61,12 +61,30 @@
   </si>
   <si>
     <t>Summe</t>
+  </si>
+  <si>
+    <t>What?</t>
+  </si>
+  <si>
+    <t>Planung</t>
+  </si>
+  <si>
+    <t>GitHub</t>
+  </si>
+  <si>
+    <t>Photoshop, Inspiration</t>
+  </si>
+  <si>
+    <t>Player Movement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;h&quot;"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -124,11 +142,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -423,18 +443,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="144" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -450,8 +471,11 @@
       <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -466,12 +490,15 @@
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="4">
         <f>D2-C2</f>
         <v>0.83333333333333393</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -486,12 +513,15 @@
         <f>21 + 20/60</f>
         <v>21.333333333333332</v>
       </c>
-      <c r="E3" s="1">
-        <f>D3-C3</f>
+      <c r="E3" s="4">
+        <f t="shared" ref="E3:E11" si="0">D3-C3</f>
         <v>2.716666666666665</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -506,497 +536,618 @@
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
-      <c r="E4" s="1">
-        <f>D4-C4</f>
+      <c r="E4" s="4">
+        <f t="shared" si="0"/>
         <v>0.83333333333333393</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45315</v>
+      </c>
+      <c r="C5" s="1">
+        <f>7+55/60</f>
+        <v>7.916666666666667</v>
+      </c>
+      <c r="D5" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>1.666666666666667</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45315</v>
+      </c>
+      <c r="C6" s="1">
+        <f>11 + 10/60</f>
+        <v>11.166666666666666</v>
+      </c>
+      <c r="D6" s="1">
+        <f xml:space="preserve"> 13</f>
+        <v>13</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" si="0"/>
+        <v>1.8333333333333339</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F7" s="1"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F8" s="1"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F11" s="1"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="4"/>
+      <c r="F12" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+      <c r="F13" s="1"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+      <c r="F14" s="1"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="4"/>
+      <c r="F15" s="1"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+      <c r="F16" s="1"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="4"/>
+      <c r="F17" s="1"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="4"/>
+      <c r="F18" s="1"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+      <c r="F19" s="1"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="4"/>
+      <c r="F20" s="1"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+      <c r="F21" s="1"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+      <c r="F22" s="1"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+      <c r="F23" s="1"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E24" s="4"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E25" s="4"/>
+      <c r="F25" s="1"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E26" s="4"/>
+      <c r="F26" s="1"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E27" s="4"/>
+      <c r="F27" s="1"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E28" s="4"/>
+      <c r="F28" s="1"/>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E29" s="4"/>
+      <c r="F29" s="1"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E30" s="4"/>
+      <c r="F30" s="1"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E31" s="4"/>
+      <c r="F31" s="1"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E32" s="4"/>
+      <c r="F32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="4"/>
+      <c r="F33" s="1"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="4"/>
+      <c r="F34" s="1"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="4"/>
+      <c r="F35" s="1"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" s="4"/>
+      <c r="F36" s="1"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E37" s="4"/>
+      <c r="F37" s="1"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E38" s="4"/>
+      <c r="F38" s="1"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E39" s="4"/>
+      <c r="F39" s="1"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E40" s="4"/>
+      <c r="F40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E41" s="4"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E42" s="4"/>
+      <c r="F42" s="1"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E43" s="4"/>
+      <c r="F43" s="1"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E44" s="4"/>
+      <c r="F44" s="1"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E45" s="4"/>
+      <c r="F45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E46" s="4"/>
+      <c r="F46" s="1"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E47" s="4"/>
+      <c r="F47" s="1"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E48" s="4"/>
+      <c r="F48" s="1"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="4"/>
+      <c r="F49" s="1"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="4"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
-      <c r="E51" s="1"/>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E51" s="4"/>
+      <c r="F51" s="1"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
-      <c r="E52" s="1"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E52" s="4"/>
+      <c r="F52" s="1"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
-      <c r="E53" s="1"/>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E53" s="4"/>
+      <c r="F53" s="1"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
-      <c r="E54" s="1"/>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E54" s="4"/>
+      <c r="F54" s="1"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
-      <c r="E55" s="1"/>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E55" s="4"/>
+      <c r="F55" s="1"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
-      <c r="E56" s="1"/>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E56" s="4"/>
+      <c r="F56" s="1"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
-      <c r="E57" s="1"/>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E57" s="4"/>
+      <c r="F57" s="1"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
-      <c r="E58" s="1"/>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E58" s="4"/>
+      <c r="F58" s="1"/>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
-      <c r="E59" s="1"/>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E59" s="4"/>
+      <c r="F59" s="1"/>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
-      <c r="E60" s="1"/>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E60" s="4"/>
+      <c r="F60" s="1"/>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
-      <c r="E61" s="1"/>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E61" s="4"/>
+      <c r="F61" s="1"/>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
-      <c r="E62" s="1"/>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E62" s="4"/>
+      <c r="F62" s="1"/>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
-      <c r="E63" s="1"/>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E63" s="4"/>
+      <c r="F63" s="1"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
-      <c r="E64" s="1"/>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E64" s="4"/>
+      <c r="F64" s="1"/>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
-      <c r="E65" s="1"/>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E65" s="4"/>
+      <c r="F65" s="1"/>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
-      <c r="E66" s="1"/>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E66" s="4"/>
+      <c r="F66" s="1"/>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
-      <c r="E67" s="1"/>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E67" s="4"/>
+      <c r="F67" s="1"/>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
-      <c r="E68" s="1"/>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E68" s="4"/>
+      <c r="F68" s="1"/>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
-      <c r="E69" s="1"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E69" s="4"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
-      <c r="E70" s="1"/>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E70" s="4"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
-      <c r="E71" s="1"/>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E71" s="4"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
-      <c r="E72" s="1"/>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E72" s="4"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
-      <c r="E73" s="1"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E73" s="4"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>7</v>
+      </c>
+      <c r="E74" s="5">
+        <f>SUM(E2:E73)</f>
+        <v>7.8833333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Player movement - improved :D (final?)
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{544DC3E9-8281-4935-B92A-A62AE4DFD7FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C245AD92-2637-4E2D-A712-5AC86B84BBEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -83,7 +83,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="#,##0.00\ &quot;h&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;h&quot;"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -147,8 +147,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -443,10 +443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F74"/>
+  <dimension ref="A1:G74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="G66" sqref="G66"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +455,7 @@
     <col min="6" max="6" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -475,7 +475,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -498,7 +498,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -514,138 +514,150 @@
         <v>21.333333333333332</v>
       </c>
       <c r="E3" s="4">
-        <f t="shared" ref="E3:E11" si="0">D3-C3</f>
+        <f>D3-C3</f>
         <v>2.716666666666665</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
         <v>45315</v>
       </c>
       <c r="C4" s="1">
+        <f>11 + 10/60</f>
+        <v>11.166666666666666</v>
+      </c>
+      <c r="D4" s="1">
+        <f xml:space="preserve"> 13</f>
+        <v>13</v>
+      </c>
+      <c r="E4" s="4">
+        <f>D4-C4</f>
+        <v>1.8333333333333339</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3">
+        <v>45315</v>
+      </c>
+      <c r="C5" s="1">
+        <f xml:space="preserve"> 17 + 30/60</f>
+        <v>17.5</v>
+      </c>
+      <c r="D5" s="1">
+        <f>18 + 40/60</f>
+        <v>18.666666666666668</v>
+      </c>
+      <c r="E5" s="4">
+        <f>D5-C5</f>
+        <v>1.1666666666666679</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="3">
+        <v>45315</v>
+      </c>
+      <c r="C6" s="1">
         <f>8 + 45/60</f>
         <v>8.75</v>
       </c>
-      <c r="D4" s="1">
+      <c r="D6" s="1">
         <f>9 + 35/60</f>
         <v>9.5833333333333339</v>
       </c>
-      <c r="E4" s="4">
-        <f t="shared" si="0"/>
+      <c r="E6" s="4">
+        <f>D6-C6</f>
         <v>0.83333333333333393</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B7" s="3">
         <v>45315</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C7" s="1">
         <f>7+55/60</f>
         <v>7.916666666666667</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D7" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
-      <c r="E5" s="4">
-        <f t="shared" si="0"/>
+      <c r="E7" s="4">
+        <f>D7-C7</f>
         <v>1.666666666666667</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="3">
-        <v>45315</v>
-      </c>
-      <c r="C6" s="1">
-        <f>11 + 10/60</f>
-        <v>11.166666666666666</v>
-      </c>
-      <c r="D6" s="1">
-        <f xml:space="preserve"> 13</f>
-        <v>13</v>
-      </c>
-      <c r="E6" s="4">
-        <f t="shared" si="0"/>
-        <v>1.8333333333333339</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="4">
-        <f t="shared" si="0"/>
+        <f>D8-C8</f>
         <v>0</v>
       </c>
       <c r="F8" s="1"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4">
-        <f t="shared" si="0"/>
+        <f>D9-C9</f>
         <v>0</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4">
-        <f t="shared" si="0"/>
+        <f>D10-C10</f>
         <v>0</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4">
-        <f t="shared" si="0"/>
+        <f>D11-C11</f>
         <v>0</v>
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -653,7 +665,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -661,7 +673,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -669,7 +681,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -677,7 +689,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1147,12 +1159,12 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>7.8833333333333337</v>
+        <v>9.0500000000000007</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E4">
-    <sortCondition ref="A2:A4"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F11">
+    <sortCondition ref="A1:A11"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
player switching + camera
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6796854-E812-45FA-8BCE-9729238FA044}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7D80C2-375E-4E17-A202-337CC330F483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
   <si>
     <t>Name</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Player Movement - verbessert</t>
+  </si>
+  <si>
+    <t>Player Swap ability +  Camera</t>
   </si>
 </sst>
 </file>
@@ -145,13 +148,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -446,19 +450,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G74"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -478,7 +482,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -494,14 +498,14 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E2" s="4">
-        <f>D2-C2</f>
+        <f t="shared" ref="E2:E11" si="0">D2-C2</f>
         <v>0.83333333333333393</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -517,14 +521,14 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E3" s="4">
-        <f>D3-C3</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333393</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -540,14 +544,15 @@
         <v>21.333333333333332</v>
       </c>
       <c r="E4" s="4">
-        <f>D4-C4</f>
+        <f t="shared" si="0"/>
         <v>2.716666666666665</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -563,7 +568,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="4">
-        <f>D5-C5</f>
+        <f t="shared" si="0"/>
         <v>1.8333333333333339</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -571,7 +576,7 @@
       </c>
       <c r="G5" s="5"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -587,7 +592,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E6" s="4">
-        <f>D6-C6</f>
+        <f t="shared" si="0"/>
         <v>1.666666666666667</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -595,7 +600,7 @@
       </c>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
@@ -611,58 +616,70 @@
         <v>18.666666666666668</v>
       </c>
       <c r="E7" s="4">
-        <f>D7-C7</f>
+        <f t="shared" si="0"/>
         <v>1.1666666666666679</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3">
+        <v>45316</v>
+      </c>
+      <c r="C8" s="1">
+        <f>19+42/60</f>
+        <v>19.7</v>
+      </c>
+      <c r="D8" s="1">
+        <f xml:space="preserve"> 21 + 30/60</f>
+        <v>21.5</v>
+      </c>
       <c r="E8" s="4">
-        <f>D8-C8</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>1.8000000000000007</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="4">
-        <f>D9-C9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F9" s="1"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="4">
-        <f>D10-C10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F10" s="1"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="4">
-        <f>D11-C11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="F11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -670,7 +687,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="1"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -678,7 +695,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="1"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -686,7 +703,7 @@
       <c r="E14" s="4"/>
       <c r="F14" s="1"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -694,7 +711,7 @@
       <c r="E15" s="4"/>
       <c r="F15" s="1"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -1164,7 +1181,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>9.0500000000000007</v>
+        <v>10.850000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix sprite flipping ;-;
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7D80C2-375E-4E17-A202-337CC330F483}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{137B5686-F2E3-4E8C-8E0F-E037FC4741E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>Player Swap ability +  Camera</t>
+  </si>
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Storyline</t>
   </si>
 </sst>
 </file>
@@ -453,7 +459,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -647,26 +653,50 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3">
+        <v>45321</v>
+      </c>
+      <c r="C9" s="1">
+        <f>8+45/60</f>
+        <v>8.75</v>
+      </c>
+      <c r="D9" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="1"/>
+        <v>0.83333333333333393</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3">
+        <v>45322</v>
+      </c>
+      <c r="C10" s="1">
+        <f>8+45/60</f>
+        <v>8.75</v>
+      </c>
+      <c r="D10" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F10" s="1"/>
+        <v>0.83333333333333393</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -1181,7 +1211,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>10.850000000000001</v>
+        <v>12.516666666666669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
goals working uwu + next scene
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2EB3D4-299B-411C-9E4C-4ABFD025581C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5639C806-41BA-41AD-AE0E-85ED604E890D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>textures</t>
+  </si>
+  <si>
+    <t>goalpoints + next level</t>
   </si>
 </sst>
 </file>
@@ -467,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,7 +516,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E2" s="4">
-        <f>D2-C2</f>
+        <f t="shared" ref="E2:E19" si="0">D2-C2</f>
         <v>0.83333333333333393</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -536,7 +539,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="E3" s="4">
-        <f>D3-C3</f>
+        <f t="shared" si="0"/>
         <v>2.716666666666665</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -559,7 +562,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E4" s="4">
-        <f>D4-C4</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333393</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -583,7 +586,7 @@
         <v>13</v>
       </c>
       <c r="E5" s="4">
-        <f>D5-C5</f>
+        <f t="shared" si="0"/>
         <v>1.8333333333333339</v>
       </c>
       <c r="F5" s="1" t="s">
@@ -607,7 +610,7 @@
         <v>18.666666666666668</v>
       </c>
       <c r="E6" s="4">
-        <f>D6-C6</f>
+        <f t="shared" si="0"/>
         <v>1.1666666666666679</v>
       </c>
       <c r="F6" s="1" t="s">
@@ -631,7 +634,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E7" s="4">
-        <f>D7-C7</f>
+        <f t="shared" si="0"/>
         <v>1.666666666666667</v>
       </c>
       <c r="F7" s="1" t="s">
@@ -654,7 +657,7 @@
         <v>21.5</v>
       </c>
       <c r="E8" s="4">
-        <f>D8-C8</f>
+        <f t="shared" si="0"/>
         <v>1.8000000000000007</v>
       </c>
       <c r="F8" s="1" t="s">
@@ -677,7 +680,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E9" s="4">
-        <f>D9-C9</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333393</v>
       </c>
       <c r="F9" s="1" t="s">
@@ -700,7 +703,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E10" s="4">
-        <f>D10-C10</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333393</v>
       </c>
       <c r="F10" s="1" t="s">
@@ -723,7 +726,7 @@
         <v>16.666666666666668</v>
       </c>
       <c r="E11" s="4">
-        <f>D11-C11</f>
+        <f t="shared" si="0"/>
         <v>1.9166666666666679</v>
       </c>
       <c r="F11" s="1" t="s">
@@ -746,7 +749,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E12" s="4">
-        <f>D12-C12</f>
+        <f t="shared" si="0"/>
         <v>1.666666666666667</v>
       </c>
       <c r="F12" s="1" t="s">
@@ -769,7 +772,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="E13" s="4">
-        <f>D13-C13</f>
+        <f t="shared" si="0"/>
         <v>1.666666666666667</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -777,19 +780,37 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="1"/>
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45323</v>
+      </c>
+      <c r="C14" s="1">
+        <f>17+35/60</f>
+        <v>17.583333333333332</v>
+      </c>
+      <c r="D14" s="1">
+        <f>19</f>
+        <v>19</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="0"/>
+        <v>1.4166666666666679</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
-      <c r="E15" s="4"/>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -797,7 +818,10 @@
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
-      <c r="E16" s="4"/>
+      <c r="E16" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -805,7 +829,10 @@
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -813,7 +840,10 @@
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
-      <c r="E18" s="4"/>
+      <c r="E18" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -821,7 +851,10 @@
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
-      <c r="E19" s="4"/>
+      <c r="E19" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1262,7 +1295,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>17.766666666666673</v>
+        <v>19.183333333333341</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
goals - coroutines -> finished :D
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5639C806-41BA-41AD-AE0E-85ED604E890D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41218EA-722B-4629-B89F-EFC9CD7A6535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>goalpoints + next level</t>
+  </si>
+  <si>
+    <t>Refactoring</t>
+  </si>
+  <si>
+    <t>goalpoints - coroutines -&gt; finished</t>
   </si>
 </sst>
 </file>
@@ -470,8 +476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,25 +554,25 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="3">
-        <v>45314</v>
+        <v>45315</v>
       </c>
       <c r="C4" s="1">
-        <f>8 + 45/60</f>
-        <v>8.75</v>
+        <f>11 + 10/60</f>
+        <v>11.166666666666666</v>
       </c>
       <c r="D4" s="1">
-        <f>9 + 35/60</f>
-        <v>9.5833333333333339</v>
+        <f xml:space="preserve"> 13</f>
+        <v>13</v>
       </c>
       <c r="E4" s="4">
         <f t="shared" si="0"/>
-        <v>0.83333333333333393</v>
+        <v>1.8333333333333339</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H4" s="6"/>
     </row>
@@ -578,19 +584,19 @@
         <v>45315</v>
       </c>
       <c r="C5" s="1">
-        <f>11 + 10/60</f>
-        <v>11.166666666666666</v>
+        <f xml:space="preserve"> 17 + 30/60</f>
+        <v>17.5</v>
       </c>
       <c r="D5" s="1">
-        <f xml:space="preserve"> 13</f>
+        <f>18 + 40/60</f>
+        <v>18.666666666666668</v>
+      </c>
+      <c r="E5" s="4">
+        <f t="shared" si="0"/>
+        <v>1.1666666666666679</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E5" s="4">
-        <f t="shared" si="0"/>
-        <v>1.8333333333333339</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="G5" s="5"/>
     </row>
@@ -599,35 +605,35 @@
         <v>4</v>
       </c>
       <c r="B6" s="3">
-        <v>45315</v>
+        <v>45316</v>
       </c>
       <c r="C6" s="1">
-        <f xml:space="preserve"> 17 + 30/60</f>
-        <v>17.5</v>
+        <f>19+42/60</f>
+        <v>19.7</v>
       </c>
       <c r="D6" s="1">
-        <f>18 + 40/60</f>
-        <v>18.666666666666668</v>
+        <f xml:space="preserve"> 21 + 30/60</f>
+        <v>21.5</v>
       </c>
       <c r="E6" s="4">
         <f t="shared" si="0"/>
-        <v>1.1666666666666679</v>
+        <v>1.8000000000000007</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G6" s="5"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3">
-        <v>45315</v>
+        <v>45322</v>
       </c>
       <c r="C7" s="1">
-        <f>7+55/60</f>
-        <v>7.916666666666667</v>
+        <f>8+45/60</f>
+        <v>8.75</v>
       </c>
       <c r="D7" s="1">
         <f>9+35/60</f>
@@ -635,45 +641,47 @@
       </c>
       <c r="E7" s="4">
         <f t="shared" si="0"/>
-        <v>1.666666666666667</v>
+        <v>0.83333333333333393</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="H7" s="5"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="3">
-        <v>45316</v>
+        <v>45322</v>
       </c>
       <c r="C8" s="1">
-        <f>19+42/60</f>
-        <v>19.7</v>
+        <f>14+45/60</f>
+        <v>14.75</v>
       </c>
       <c r="D8" s="1">
-        <f xml:space="preserve"> 21 + 30/60</f>
-        <v>21.5</v>
+        <f>16+40/60</f>
+        <v>16.666666666666668</v>
       </c>
       <c r="E8" s="4">
         <f t="shared" si="0"/>
-        <v>1.8000000000000007</v>
+        <v>1.9166666666666679</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H8" s="5"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B9" s="3">
-        <v>45321</v>
+        <v>45323</v>
       </c>
       <c r="C9" s="1">
-        <f>8+45/60</f>
-        <v>8.75</v>
+        <f>7+55/60</f>
+        <v>7.916666666666667</v>
       </c>
       <c r="D9" s="1">
         <f>9+35/60</f>
@@ -681,33 +689,34 @@
       </c>
       <c r="E9" s="4">
         <f t="shared" si="0"/>
-        <v>0.83333333333333393</v>
+        <v>1.666666666666667</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="3">
-        <v>45322</v>
+        <v>45323</v>
       </c>
       <c r="C10" s="1">
-        <f>8+45/60</f>
-        <v>8.75</v>
+        <f>17+35/60</f>
+        <v>17.583333333333332</v>
       </c>
       <c r="D10" s="1">
-        <f>9+35/60</f>
-        <v>9.5833333333333339</v>
+        <f>19</f>
+        <v>19</v>
       </c>
       <c r="E10" s="4">
         <f t="shared" si="0"/>
-        <v>0.83333333333333393</v>
+        <v>1.4166666666666679</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -715,114 +724,138 @@
         <v>4</v>
       </c>
       <c r="B11" s="3">
-        <v>45322</v>
+        <v>45324</v>
       </c>
       <c r="C11" s="1">
-        <f>14+45/60</f>
-        <v>14.75</v>
+        <f>8+45/60</f>
+        <v>8.75</v>
       </c>
       <c r="D11" s="1">
-        <f>16+40/60</f>
-        <v>16.666666666666668</v>
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
       </c>
       <c r="E11" s="4">
         <f t="shared" si="0"/>
-        <v>1.9166666666666679</v>
+        <v>0.83333333333333393</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="3">
+        <v>45324</v>
+      </c>
+      <c r="C12" s="1">
+        <f>13+53/60</f>
+        <v>13.883333333333333</v>
+      </c>
+      <c r="D12" s="1">
+        <f>14+36/60</f>
+        <v>14.6</v>
+      </c>
+      <c r="E12" s="4">
+        <f t="shared" si="0"/>
+        <v>0.71666666666666679</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3">
-        <v>45322</v>
-      </c>
-      <c r="C12" s="1">
+      <c r="B13" s="3">
+        <v>45314</v>
+      </c>
+      <c r="C13" s="1">
+        <f>8 + 45/60</f>
+        <v>8.75</v>
+      </c>
+      <c r="D13" s="1">
+        <f>9 + 35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333393</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3">
+        <v>45315</v>
+      </c>
+      <c r="C14" s="1">
         <f>7+55/60</f>
         <v>7.916666666666667</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D14" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E14" s="4">
         <f t="shared" si="0"/>
         <v>1.666666666666667</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="3">
-        <v>45323</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3">
+        <v>45321</v>
+      </c>
+      <c r="C15" s="1">
+        <f>8+45/60</f>
+        <v>8.75</v>
+      </c>
+      <c r="D15" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="0"/>
+        <v>0.83333333333333393</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3">
+        <v>45322</v>
+      </c>
+      <c r="C16" s="1">
         <f>7+55/60</f>
         <v>7.916666666666667</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D16" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E16" s="4">
         <f t="shared" si="0"/>
         <v>1.666666666666667</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="3">
-        <v>45323</v>
-      </c>
-      <c r="C14" s="1">
-        <f>17+35/60</f>
-        <v>17.583333333333332</v>
-      </c>
-      <c r="D14" s="1">
-        <f>19</f>
+      <c r="F16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="4">
-        <f t="shared" si="0"/>
-        <v>1.4166666666666679</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
@@ -1295,12 +1328,12 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>19.183333333333341</v>
+        <v>20.733333333333338</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F13">
-    <sortCondition ref="B2:B13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F19">
+    <sortCondition ref="A16:A19"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
animation refactor ( i love refactoring for the sake of readability and easiness)
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -5,16 +5,15 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F41218EA-722B-4629-B89F-EFC9CD7A6535}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FB8963-D511-4186-AAC1-604C176BC187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId1"/>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId2"/>
+    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -106,6 +105,9 @@
   </si>
   <si>
     <t>goalpoints - coroutines -&gt; finished</t>
+  </si>
+  <si>
+    <t>refactor animation -&gt; slip jumping and falling + merged playerMovement and animController</t>
   </si>
 </sst>
 </file>
@@ -459,25 +461,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B658D80B-CFF5-4360-B741-6C8515FE1FEE}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,15 +846,27 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
+      <c r="A17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="3">
+        <v>45326</v>
+      </c>
+      <c r="C17" s="1">
+        <f xml:space="preserve"> 18+30/60</f>
+        <v>18.5</v>
+      </c>
+      <c r="D17" s="1">
+        <f>19+42/60</f>
+        <v>19.7</v>
+      </c>
       <c r="E17" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="1"/>
+        <v>1.1999999999999993</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>20.733333333333338</v>
+        <v>21.933333333333337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
button input working -> no event link yet
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54FB8963-D511-4186-AAC1-604C176BC187}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE35316-2BF3-4D19-8AA4-E67A6FF77C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3030" yWindow="3030" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Name</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>refactor animation -&gt; slip jumping and falling + merged playerMovement and animController</t>
+  </si>
+  <si>
+    <t>Arsi</t>
+  </si>
+  <si>
+    <t>Button input working -&gt; no even link</t>
   </si>
 </sst>
 </file>
@@ -464,8 +470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -869,15 +875,27 @@
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
+      <c r="A18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="3">
+        <v>45334</v>
+      </c>
+      <c r="C18" s="1">
+        <f>10+21/60</f>
+        <v>10.35</v>
+      </c>
+      <c r="D18" s="1">
+        <f>10+42/60</f>
+        <v>10.7</v>
+      </c>
       <c r="E18" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18" s="1"/>
+        <v>0.34999999999999964</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1328,7 +1346,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>21.933333333333337</v>
+        <v>22.283333333333339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
button event link start
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BE35316-2BF3-4D19-8AA4-E67A6FF77C87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B6F3C8A-0C2F-47A1-B412-C915EBFB1C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="27">
   <si>
     <t>Name</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Button input working -&gt; no even link</t>
+  </si>
+  <si>
+    <t>Button even link</t>
   </si>
 </sst>
 </file>
@@ -471,7 +474,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,15 +901,27 @@
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
+      <c r="A19" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="3">
+        <v>45334</v>
+      </c>
+      <c r="C19" s="1">
+        <f>12+53/60</f>
+        <v>12.883333333333333</v>
+      </c>
+      <c r="D19" s="1">
+        <f>13+7/60</f>
+        <v>13.116666666666667</v>
+      </c>
       <c r="E19" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F19" s="1"/>
+        <v>0.23333333333333428</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
@@ -1346,7 +1361,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>22.283333333333339</v>
+        <v>22.516666666666673</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
button event (move) finally working
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D253D86-918A-4F52-A82B-705F03A24D98}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6CCD613-FB9A-4B21-B42D-212ADF3B2731}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -480,7 +480,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -957,7 +957,7 @@
         <v>6</v>
       </c>
       <c r="B21" s="3">
-        <v>45336</v>
+        <v>45335</v>
       </c>
       <c r="C21" s="1">
         <f>8+5/60</f>
@@ -976,13 +976,20 @@
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
+      <c r="A22" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3">
+        <v>45335</v>
+      </c>
+      <c r="C22" s="1">
+        <f>14+32/60</f>
+        <v>14.533333333333333</v>
+      </c>
       <c r="D22" s="1"/>
       <c r="E22" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-14.533333333333333</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1448,7 +1455,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>25.516666666666673</v>
+        <v>10.98333333333334</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
timelog and to pull the merge
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F22394E2-38A8-4EBA-8B6D-C62129EDE7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7431BB-040F-4BE4-AEE8-338DC5C49272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
   <si>
     <t>Name</t>
   </si>
@@ -483,7 +483,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1025,24 +1025,44 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
+      <c r="A24" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="3">
+        <v>45336</v>
+      </c>
+      <c r="C24" s="1">
+        <f>8+7/60</f>
+        <v>8.1166666666666671</v>
+      </c>
+      <c r="D24" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="E24" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4666666666666668</v>
       </c>
       <c r="F24" s="1"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
+      <c r="A25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" s="3">
+        <v>45336</v>
+      </c>
+      <c r="C25" s="1">
+        <f>8+7/60</f>
+        <v>8.1166666666666671</v>
+      </c>
+      <c r="D25" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="E25" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.4666666666666668</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -1475,7 +1495,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>26.350000000000009</v>
+        <v>29.283333333333346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
gates finally working, translationa and rotation
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7431BB-040F-4BE4-AEE8-338DC5C49272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D59225F1-0D1B-4A8E-BD02-34CC647B21DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="31">
   <si>
     <t>Name</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>gates</t>
+  </si>
+  <si>
+    <t>Sprites</t>
   </si>
 </sst>
 </file>
@@ -483,12 +486,13 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="28.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1067,26 +1071,48 @@
       <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
+      <c r="A26" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C26" s="1">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="D26" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="E26" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5833333333333339</v>
       </c>
       <c r="F26" s="1"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="3">
+        <v>45342</v>
+      </c>
+      <c r="C27" s="1">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="D27" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="E27" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="1"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
@@ -1495,7 +1521,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>29.283333333333346</v>
+        <v>32.450000000000017</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completely migrated project - started on shaders
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D87A7E-8D24-4F59-A396-7954237CD66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C49C0-333B-4CEE-9BEC-0E6C428AED6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1046,7 +1046,7 @@
         <v>8.1166666666666671</v>
       </c>
       <c r="D24" s="1">
-        <f>9+35/60</f>
+        <f t="shared" ref="D24:D31" si="1">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="E24" s="4">
@@ -1067,7 +1067,7 @@
         <v>8.1166666666666671</v>
       </c>
       <c r="D25" s="1">
-        <f>9+35/60</f>
+        <f t="shared" si="1"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="E25" s="4">
@@ -1090,7 +1090,7 @@
         <v>8</v>
       </c>
       <c r="D26" s="1">
-        <f>9+35/60</f>
+        <f t="shared" si="1"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="E26" s="4">
@@ -1113,7 +1113,7 @@
         <v>8</v>
       </c>
       <c r="D27" s="1">
-        <f>9+35/60</f>
+        <f t="shared" si="1"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="E27" s="4">
@@ -1136,7 +1136,7 @@
         <v>8</v>
       </c>
       <c r="D28" s="1">
-        <f>9+35/60</f>
+        <f t="shared" si="1"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="E28" s="4">
@@ -1159,7 +1159,7 @@
         <v>8</v>
       </c>
       <c r="D29" s="1">
-        <f>9+35/60</f>
+        <f t="shared" si="1"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="E29" s="4">
@@ -1171,24 +1171,44 @@
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
+      <c r="A30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B30" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C30" s="1">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="D30" s="1">
+        <f t="shared" si="1"/>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="E30" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5833333333333339</v>
       </c>
       <c r="F30" s="1"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
+      <c r="A31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="3">
+        <v>45349</v>
+      </c>
+      <c r="C31" s="1">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="D31" s="1">
+        <f t="shared" si="1"/>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="E31" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.5833333333333339</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -1555,7 +1575,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>35.616666666666688</v>
+        <v>38.78333333333336</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fade out animation level end
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D9C49C0-333B-4CEE-9BEC-0E6C428AED6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EA2F097-D6FB-442F-B268-C1F8B7A6DB33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3030" yWindow="3030" windowWidth="28800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -491,8 +491,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,13 +1213,23 @@
       <c r="F31" s="1"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
+      <c r="A32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="3">
+        <v>45350</v>
+      </c>
+      <c r="C32" s="1">
+        <f>18+24/60</f>
+        <v>18.399999999999999</v>
+      </c>
+      <c r="D32" s="1">
+        <f>20+21/60</f>
+        <v>20.350000000000001</v>
+      </c>
       <c r="E32" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.9500000000000028</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1575,7 +1585,7 @@
       </c>
       <c r="E74" s="5">
         <f>SUM(E2:E73)</f>
-        <v>38.78333333333336</v>
+        <v>40.733333333333363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
goal shader -> pretty good :D
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5657F5C-7590-42FE-9AAF-F9BEC6F5E0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C019833E-F166-4EBC-B3CF-311CF7F92A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t>Begin</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>finish level = cant move, goal shader testing</t>
+  </si>
+  <si>
+    <t>goal shader -&gt; pretty good :D</t>
   </si>
 </sst>
 </file>
@@ -172,7 +175,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -195,18 +198,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -488,9 +504,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="128" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -571,7 +587,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="D3" s="3">
-        <f>C3-B3</f>
+        <f t="shared" ref="D3:D26" si="0">C3-B3</f>
         <v>0.83333333333333393</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -589,7 +605,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="M3" s="3">
-        <f t="shared" ref="M3:M11" si="0">L3-K3</f>
+        <f t="shared" ref="M3:M24" si="1">L3-K3</f>
         <v>0.83333333333333393</v>
       </c>
       <c r="N3" s="1" t="s">
@@ -601,11 +617,11 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M3:M11)</f>
-        <v>12.71666666666667</v>
+        <v>12.750000000000005</v>
       </c>
       <c r="V3" s="5">
         <f>U3/(U3+U4)</f>
-        <v>0.30134281200631902</v>
+        <v>0.30106257378984641</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -621,7 +637,7 @@
         <v>21.333333333333332</v>
       </c>
       <c r="D4" s="3">
-        <f>C4-B4</f>
+        <f t="shared" si="0"/>
         <v>2.716666666666665</v>
       </c>
       <c r="E4" s="1" t="s">
@@ -632,16 +648,16 @@
         <v>45315</v>
       </c>
       <c r="K4" s="1">
-        <f>7+55/60</f>
-        <v>7.916666666666667</v>
+        <f>8</f>
+        <v>8</v>
       </c>
       <c r="L4" s="1">
-        <f t="shared" ref="L4:L11" si="1">9+35/60</f>
+        <f t="shared" ref="L4:L11" si="2">9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" si="0"/>
-        <v>1.666666666666667</v>
+        <f t="shared" si="1"/>
+        <v>1.5833333333333339</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>8</v>
@@ -651,11 +667,11 @@
       </c>
       <c r="U4" s="4">
         <f>SUM(D3:D25)</f>
-        <v>29.483333333333356</v>
+        <v>29.600000000000023</v>
       </c>
       <c r="V4" s="5">
         <f>U4/(U3+U4)</f>
-        <v>0.69865718799368104</v>
+        <v>0.69893742621015353</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -671,7 +687,7 @@
         <v>13</v>
       </c>
       <c r="D5" s="3">
-        <f>C5-B5</f>
+        <f t="shared" si="0"/>
         <v>1.8333333333333339</v>
       </c>
       <c r="E5" s="1" t="s">
@@ -685,11 +701,11 @@
         <v>8.75</v>
       </c>
       <c r="L5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83333333333333393</v>
       </c>
       <c r="N5" s="1" t="s">
@@ -709,7 +725,7 @@
         <v>18.666666666666668</v>
       </c>
       <c r="D6" s="3">
-        <f>C6-B6</f>
+        <f t="shared" si="0"/>
         <v>1.1666666666666679</v>
       </c>
       <c r="E6" s="1" t="s">
@@ -719,16 +735,15 @@
         <v>45322</v>
       </c>
       <c r="K6" s="1">
-        <f>7+55/60</f>
-        <v>7.916666666666667</v>
+        <v>8</v>
       </c>
       <c r="L6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="M6" s="3">
-        <f t="shared" si="0"/>
-        <v>1.666666666666667</v>
+        <f t="shared" si="1"/>
+        <v>1.5833333333333339</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>16</v>
@@ -747,7 +762,7 @@
         <v>21.5</v>
       </c>
       <c r="D7" s="3">
-        <f>C7-B7</f>
+        <f t="shared" si="0"/>
         <v>1.8000000000000007</v>
       </c>
       <c r="E7" s="1" t="s">
@@ -757,16 +772,15 @@
         <v>45335</v>
       </c>
       <c r="K7" s="1">
-        <f>8+5/60</f>
-        <v>8.0833333333333339</v>
+        <v>8</v>
       </c>
       <c r="L7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="M7" s="3">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <f t="shared" si="1"/>
+        <v>1.5833333333333339</v>
       </c>
       <c r="N7" s="1" t="s">
         <v>24</v>
@@ -785,7 +799,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="D8" s="3">
-        <f>C8-B8</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333393</v>
       </c>
       <c r="E8" s="1" t="s">
@@ -795,16 +809,15 @@
         <v>45336</v>
       </c>
       <c r="K8" s="1">
-        <f>8+7/60</f>
-        <v>8.1166666666666671</v>
+        <v>8</v>
       </c>
       <c r="L8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="M8" s="3">
-        <f t="shared" si="0"/>
-        <v>1.4666666666666668</v>
+        <f t="shared" si="1"/>
+        <v>1.5833333333333339</v>
       </c>
       <c r="N8" s="1" t="s">
         <v>26</v>
@@ -823,7 +836,7 @@
         <v>16.666666666666668</v>
       </c>
       <c r="D9" s="3">
-        <f>C9-B9</f>
+        <f t="shared" si="0"/>
         <v>1.9166666666666679</v>
       </c>
       <c r="E9" s="1" t="s">
@@ -837,11 +850,11 @@
         <v>8</v>
       </c>
       <c r="L9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="M9" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="N9" s="1" t="s">
@@ -853,16 +866,15 @@
         <v>45323</v>
       </c>
       <c r="B10" s="1">
-        <f>7+55/60</f>
-        <v>7.916666666666667</v>
+        <v>8</v>
       </c>
       <c r="C10" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="D10" s="3">
-        <f>C10-B10</f>
-        <v>1.666666666666667</v>
+        <f t="shared" si="0"/>
+        <v>1.5833333333333339</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>15</v>
@@ -875,11 +887,11 @@
         <v>8</v>
       </c>
       <c r="L10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="M10" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="N10" s="1" t="s">
@@ -899,7 +911,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="3">
-        <f>C11-B11</f>
+        <f t="shared" si="0"/>
         <v>1.4166666666666679</v>
       </c>
       <c r="E11" s="1" t="s">
@@ -913,11 +925,11 @@
         <v>8</v>
       </c>
       <c r="L11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>9.5833333333333339</v>
       </c>
       <c r="M11" s="3">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="N11" s="1"/>
@@ -935,11 +947,25 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="D12" s="3">
-        <f>C12-B12</f>
+        <f t="shared" si="0"/>
         <v>0.83333333333333393</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="J12" s="6">
+        <v>45356</v>
+      </c>
+      <c r="K12">
+        <v>8</v>
+      </c>
+      <c r="L12" s="7">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="M12" s="3">
+        <f t="shared" si="1"/>
+        <v>1.5833333333333339</v>
       </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
@@ -955,11 +981,15 @@
         <v>14.6</v>
       </c>
       <c r="D13" s="3">
-        <f>C13-B13</f>
+        <f t="shared" si="0"/>
         <v>0.71666666666666679</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>19</v>
+      </c>
+      <c r="M13" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -975,11 +1005,15 @@
         <v>19.7</v>
       </c>
       <c r="D14" s="3">
-        <f>C14-B14</f>
+        <f t="shared" si="0"/>
         <v>1.1999999999999993</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>20</v>
+      </c>
+      <c r="M14" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
@@ -995,11 +1029,15 @@
         <v>13.116666666666667</v>
       </c>
       <c r="D15" s="3">
-        <f>C15-B15</f>
+        <f t="shared" si="0"/>
         <v>0.23333333333333428</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="M15" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
@@ -1015,34 +1053,41 @@
         <v>10.7</v>
       </c>
       <c r="D16" s="3">
-        <f>C16-B16</f>
+        <f t="shared" si="0"/>
         <v>0.34999999999999964</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M16" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45335</v>
       </c>
       <c r="B17" s="1">
-        <f>8+5/60</f>
-        <v>8.0833333333333339</v>
+        <v>8</v>
       </c>
       <c r="C17" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="D17" s="3">
-        <f>C17-B17</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>1.5833333333333339</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M17" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45335</v>
       </c>
@@ -1055,14 +1100,18 @@
         <v>15.166666666666666</v>
       </c>
       <c r="D18" s="3">
-        <f>C18-B18</f>
+        <f t="shared" si="0"/>
         <v>0.63333333333333286</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M18" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45335</v>
       </c>
@@ -1075,32 +1124,39 @@
         <v>17.783333333333335</v>
       </c>
       <c r="D19" s="3">
-        <f>C19-B19</f>
+        <f t="shared" si="0"/>
         <v>0.20000000000000284</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M19" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45336</v>
       </c>
       <c r="B20" s="1">
-        <f>8+7/60</f>
-        <v>8.1166666666666671</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
       <c r="D20" s="3">
-        <f>C20-B20</f>
-        <v>1.4666666666666668</v>
+        <f t="shared" si="0"/>
+        <v>1.5833333333333339</v>
       </c>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M20" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45342</v>
       </c>
@@ -1113,14 +1169,18 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="D21" s="3">
-        <f>C21-B21</f>
+        <f t="shared" si="0"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M21" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45343</v>
       </c>
@@ -1133,14 +1193,18 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="D22" s="3">
-        <f>C22-B22</f>
+        <f t="shared" si="0"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M22" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45349</v>
       </c>
@@ -1153,12 +1217,16 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="D23" s="3">
-        <f>C23-B23</f>
+        <f t="shared" si="0"/>
         <v>1.5833333333333339</v>
       </c>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M23" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45350</v>
       </c>
@@ -1171,12 +1239,16 @@
         <v>20.350000000000001</v>
       </c>
       <c r="D24" s="3">
-        <f>C24-B24</f>
+        <f t="shared" si="0"/>
         <v>1.9500000000000028</v>
       </c>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="M24" s="3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45352</v>
       </c>
@@ -1189,11 +1261,31 @@
         <v>16.366666666666667</v>
       </c>
       <c r="D25" s="3">
-        <f>C25-B25</f>
+        <f t="shared" si="0"/>
         <v>1.4666666666666668</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="6">
+        <v>45356</v>
+      </c>
+      <c r="B26">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="C26">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="0"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ui buttons and first build test
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A847E20-40DD-470B-984E-593A3379AF0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D2C8D2-ED74-4B97-B108-2980996B92FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>Begin</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>some fixes</t>
+  </si>
+  <si>
+    <t>UI buttons working and first build test</t>
   </si>
 </sst>
 </file>
@@ -511,10 +514,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V29"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,7 +631,7 @@
       </c>
       <c r="V3" s="5">
         <f>U3/(U3+U4)</f>
-        <v>0.29665401862711266</v>
+        <v>0.29381619405534665</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -674,11 +677,11 @@
       </c>
       <c r="U4" s="4">
         <f>SUM(D3:D100)</f>
-        <v>33.983333333333363</v>
+        <v>34.450000000000031</v>
       </c>
       <c r="V4" s="5">
         <f>U4/(U3+U4)</f>
-        <v>0.70334598137288729</v>
+        <v>0.70618380594465324</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1353,8 +1356,28 @@
         <f>C29-B29</f>
         <v>0.60000000000000142</v>
       </c>
-      <c r="E29" s="8" t="s">
+      <c r="E29" s="7" t="s">
         <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
+        <v>45361</v>
+      </c>
+      <c r="B30">
+        <f>16+42/60</f>
+        <v>16.7</v>
+      </c>
+      <c r="C30">
+        <f>17+10/60</f>
+        <v>17.166666666666668</v>
+      </c>
+      <c r="D30" s="3">
+        <f>C30-B30</f>
+        <v>0.46666666666666856</v>
+      </c>
+      <c r="E30" s="8" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
main menu, jumppad and spike
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\programming projects\Unity\Projects\the-ol-switcheroo\Buerokratie\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5D2C8D2-ED74-4B97-B108-2980996B92FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49404491-FADF-49A5-8879-F36EB9645A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="39">
   <si>
     <t>Begin</t>
   </si>
@@ -150,6 +150,9 @@
   </si>
   <si>
     <t>UI buttons working and first build test</t>
+  </si>
+  <si>
+    <t>Main menu, jumppad and spike</t>
   </si>
 </sst>
 </file>
@@ -514,10 +517,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V30"/>
+  <dimension ref="A1:V31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,11 +630,11 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M3:M100)</f>
-        <v>14.333333333333339</v>
+        <v>15.916666666666673</v>
       </c>
       <c r="V3" s="5">
         <f>U3/(U3+U4)</f>
-        <v>0.29381619405534665</v>
+        <v>0.30638434392043623</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -677,11 +680,11 @@
       </c>
       <c r="U4" s="4">
         <f>SUM(D3:D100)</f>
-        <v>34.450000000000031</v>
+        <v>36.033333333333367</v>
       </c>
       <c r="V4" s="5">
         <f>U4/(U3+U4)</f>
-        <v>0.70618380594465324</v>
+        <v>0.69361565607956377</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -942,7 +945,9 @@
         <f t="shared" si="1"/>
         <v>1.5833333333333339</v>
       </c>
-      <c r="N11" s="1"/>
+      <c r="N11" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
@@ -977,6 +982,9 @@
         <f t="shared" si="1"/>
         <v>1.5833333333333339</v>
       </c>
+      <c r="N12" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="13" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
@@ -997,11 +1005,23 @@
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="L13" s="7"/>
+      <c r="J13" s="6">
+        <v>45363</v>
+      </c>
+      <c r="K13">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="L13" s="7">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="M13" s="3">
         <f t="shared" ref="M13" si="3">L13-K13</f>
-        <v>0</v>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:22" x14ac:dyDescent="0.25">
@@ -1023,6 +1043,7 @@
       <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="J14" s="6"/>
       <c r="M14" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1047,6 +1068,7 @@
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="J15" s="6"/>
       <c r="M15" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1071,6 +1093,7 @@
       <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="J16" s="6"/>
       <c r="M16" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1094,6 +1117,7 @@
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="J17" s="6"/>
       <c r="M17" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1118,6 +1142,7 @@
       <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="J18" s="6"/>
       <c r="M18" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1142,6 +1167,7 @@
       <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="J19" s="6"/>
       <c r="M19" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1163,6 +1189,7 @@
         <v>1.5833333333333339</v>
       </c>
       <c r="E20" s="1"/>
+      <c r="J20" s="6"/>
       <c r="M20" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1187,6 +1214,7 @@
       <c r="E21" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="J21" s="6"/>
       <c r="M21" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1211,6 +1239,7 @@
       <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="J22" s="6"/>
       <c r="M22" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1233,6 +1262,7 @@
         <v>1.5833333333333339</v>
       </c>
       <c r="E23" s="1"/>
+      <c r="J23" s="6"/>
       <c r="M23" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1255,6 +1285,7 @@
         <v>1.9500000000000028</v>
       </c>
       <c r="E24" s="1"/>
+      <c r="J24" s="6"/>
       <c r="M24" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -1279,6 +1310,7 @@
       <c r="E25" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="J25" s="6"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
@@ -1299,6 +1331,7 @@
       <c r="E26" s="7" t="s">
         <v>34</v>
       </c>
+      <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
@@ -1319,6 +1352,7 @@
       <c r="E27" s="7" t="s">
         <v>35</v>
       </c>
+      <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
@@ -1376,8 +1410,28 @@
         <f>C30-B30</f>
         <v>0.46666666666666856</v>
       </c>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="7" t="s">
         <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="6">
+        <v>45363</v>
+      </c>
+      <c r="B31">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="C31">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="D31" s="3">
+        <f>C31-B31</f>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactoring and level editing in PS
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49404491-FADF-49A5-8879-F36EB9645A1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{775C7878-D1C2-49DA-AE20-55525D5AD6CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -187,7 +187,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -210,23 +210,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -234,8 +223,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -517,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V31"/>
+  <dimension ref="A1:V32"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -630,11 +617,11 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M3:M100)</f>
-        <v>15.916666666666673</v>
+        <v>17.500000000000007</v>
       </c>
       <c r="V3" s="5">
         <f>U3/(U3+U4)</f>
-        <v>0.30638434392043623</v>
+        <v>0.32689912826899115</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -684,7 +671,7 @@
       </c>
       <c r="V4" s="5">
         <f>U4/(U3+U4)</f>
-        <v>0.69361565607956377</v>
+        <v>0.67310087173100885</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -968,13 +955,13 @@
       <c r="E12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J12" s="6">
+      <c r="J12" s="2">
         <v>45356</v>
       </c>
-      <c r="K12">
-        <v>8</v>
-      </c>
-      <c r="L12" s="7">
+      <c r="K12" s="1">
+        <v>8</v>
+      </c>
+      <c r="L12" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1005,14 +992,14 @@
       <c r="E13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="2">
         <v>45363</v>
       </c>
-      <c r="K13">
+      <c r="K13" s="1">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="L13" s="7">
+      <c r="L13" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1043,11 +1030,22 @@
       <c r="E14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J14" s="6"/>
+      <c r="J14" s="2">
+        <v>45384</v>
+      </c>
+      <c r="K14" s="1">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="L14" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="M14" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="N14" s="1"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
@@ -1068,11 +1066,14 @@
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="6"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
       <c r="M15" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="N15" s="1"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1093,13 +1094,16 @@
       <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="6"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
       <c r="M16" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>45335</v>
       </c>
@@ -1117,13 +1121,16 @@
       <c r="E17" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J17" s="6"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
       <c r="M17" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N17" s="1"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>45335</v>
       </c>
@@ -1142,13 +1149,16 @@
       <c r="E18" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J18" s="6"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
       <c r="M18" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N18" s="1"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>45335</v>
       </c>
@@ -1167,13 +1177,16 @@
       <c r="E19" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="J19" s="6"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
       <c r="M19" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N19" s="1"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>45336</v>
       </c>
@@ -1189,13 +1202,16 @@
         <v>1.5833333333333339</v>
       </c>
       <c r="E20" s="1"/>
-      <c r="J20" s="6"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
       <c r="M20" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N20" s="1"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>45342</v>
       </c>
@@ -1214,13 +1230,16 @@
       <c r="E21" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J21" s="6"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
       <c r="M21" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N21" s="1"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>45343</v>
       </c>
@@ -1239,13 +1258,16 @@
       <c r="E22" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J22" s="6"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
       <c r="M22" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N22" s="1"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>45349</v>
       </c>
@@ -1262,13 +1284,16 @@
         <v>1.5833333333333339</v>
       </c>
       <c r="E23" s="1"/>
-      <c r="J23" s="6"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
       <c r="M23" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N23" s="1"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>45350</v>
       </c>
@@ -1285,13 +1310,16 @@
         <v>1.9500000000000028</v>
       </c>
       <c r="E24" s="1"/>
-      <c r="J24" s="6"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
       <c r="M24" s="3">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="N24" s="1"/>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>45352</v>
       </c>
@@ -1312,15 +1340,15 @@
       </c>
       <c r="J25" s="6"/>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="6">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
         <v>45356</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="1">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1328,20 +1356,20 @@
         <f t="shared" si="0"/>
         <v>1.5833333333333339</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="1" t="s">
         <v>34</v>
       </c>
       <c r="J26" s="6"/>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="6">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
         <v>45357</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="1">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1349,20 +1377,20 @@
         <f>C27-B27</f>
         <v>1.5833333333333339</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="E27" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J27" s="6"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="6">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
         <v>45357</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="1">
         <f>17+54/60</f>
         <v>17.899999999999999</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="1">
         <f>18+31/60</f>
         <v>18.516666666666666</v>
       </c>
@@ -1370,19 +1398,19 @@
         <f>C28-B28</f>
         <v>0.61666666666666714</v>
       </c>
-      <c r="E28" s="7" t="s">
+      <c r="E28" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="6">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
         <v>45359</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="1">
         <f>15+53/60</f>
         <v>15.883333333333333</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="1">
         <f>16+29/60</f>
         <v>16.483333333333334</v>
       </c>
@@ -1390,19 +1418,19 @@
         <f>C29-B29</f>
         <v>0.60000000000000142</v>
       </c>
-      <c r="E29" s="7" t="s">
+      <c r="E29" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="6">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
         <v>45361</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="1">
         <f>16+42/60</f>
         <v>16.7</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="1">
         <f>17+10/60</f>
         <v>17.166666666666668</v>
       </c>
@@ -1410,19 +1438,19 @@
         <f>C30-B30</f>
         <v>0.46666666666666856</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="E30" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="6">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>45363</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="1">
         <f>8</f>
         <v>8</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="1">
         <f>9+35/60</f>
         <v>9.5833333333333339</v>
       </c>
@@ -1430,9 +1458,24 @@
         <f>C31-B31</f>
         <v>1.5833333333333339</v>
       </c>
-      <c r="E31" s="8" t="s">
+      <c r="E31" s="1" t="s">
         <v>38</v>
       </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>45384</v>
+      </c>
+      <c r="B32" s="1">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="C32" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="1"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A3:E25">

</xml_diff>

<commit_message>
level 1 and 2 built
</commit_message>
<xml_diff>
--- a/Buerokratie/timeLog.xlsx
+++ b/Buerokratie/timeLog.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\programmingProjects\SWP\the 'ol switcheroo\Buerokratie\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77A4092-1DD7-4C2E-B423-63745F51B75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43A163A-6F3D-46DE-85D5-D6058EDB8FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Begin</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Level designing in PS</t>
+  </si>
+  <si>
+    <t>Level designs implementieren</t>
   </si>
 </sst>
 </file>
@@ -232,7 +235,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -244,6 +247,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Prozent" xfId="1" builtinId="5"/>
@@ -525,15 +529,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V33"/>
+  <dimension ref="A1:V34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="274" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T1" sqref="T1"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="88.42578125" bestFit="1" customWidth="1"/>
@@ -639,11 +643,11 @@
       </c>
       <c r="U3" s="4">
         <f>SUM(M3:M100)</f>
-        <v>19.083333333333343</v>
+        <v>20.666666666666679</v>
       </c>
       <c r="V3" s="5">
         <f>U3/(U3+U4)</f>
-        <v>0.32742350586216745</v>
+        <v>0.33631678871711407</v>
       </c>
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
@@ -689,11 +693,11 @@
       </c>
       <c r="U4" s="4">
         <f>SUM(D3:D100)</f>
-        <v>39.200000000000038</v>
+        <v>40.783333333333374</v>
       </c>
       <c r="V4" s="5">
         <f>U4/(U3+U4)</f>
-        <v>0.67257649413783249</v>
+        <v>0.66368321128288588</v>
       </c>
     </row>
     <row r="5" spans="1:22" x14ac:dyDescent="0.25">
@@ -1105,7 +1109,9 @@
         <f t="shared" si="1"/>
         <v>1.5833333333333339</v>
       </c>
-      <c r="N15" s="1"/>
+      <c r="N15" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
@@ -1126,14 +1132,24 @@
       <c r="E16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J16" s="2"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
+      <c r="J16" s="2">
+        <v>45391</v>
+      </c>
+      <c r="K16" s="1">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="L16" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
       <c r="M16" s="3">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N16" s="1"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
@@ -1406,7 +1422,7 @@
         <v>9.5833333333333339</v>
       </c>
       <c r="D27" s="3">
-        <f t="shared" ref="D27:D33" si="4">C27-B27</f>
+        <f t="shared" ref="D27:D34" si="4">C27-B27</f>
         <v>1.5833333333333339</v>
       </c>
       <c r="E27" s="1" t="s">
@@ -1532,6 +1548,26 @@
       </c>
       <c r="E33" s="7" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="6">
+        <v>45391</v>
+      </c>
+      <c r="B34">
+        <f>8</f>
+        <v>8</v>
+      </c>
+      <c r="C34" s="1">
+        <f>9+35/60</f>
+        <v>9.5833333333333339</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="4"/>
+        <v>1.5833333333333339</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>